<commit_message>
📊 Horarios actualizados Línea 141 - 1179
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -437,7 +437,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:04:01</t>
+          <t>Última actualización: 02:13:42</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:04:01</t>
+          <t>02:13:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>03:09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,12 +503,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:04:01</t>
+          <t>02:13:42</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:55</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:04:01</t>
+          <t>02:13:42</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -561,7 +561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,14 +579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:04:01</t>
+          <t>Última actualización: 02:13:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 1</t>
         </is>
       </c>
     </row>
@@ -620,12 +620,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:04:01</t>
+          <t>02:13:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>03:09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -634,34 +634,9 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>01:04:01</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>02:58</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>114</v>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -696,7 +671,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:04:01</t>
+          <t>Última actualización: 02:13:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1180
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:13:42</t>
+          <t>Última actualización: 03:02:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:13:42</t>
+          <t>03:02:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:09</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:13:42</t>
+          <t>03:02:37</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:55</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,23 +528,48 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:13:42</t>
+          <t>03:02:37</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03:02:37</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>111</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -579,7 +604,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:13:42</t>
+          <t>Última actualización: 03:02:37</t>
         </is>
       </c>
     </row>
@@ -620,21 +645,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:13:42</t>
+          <t>03:02:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:09</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -671,7 +696,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:13:42</t>
+          <t>Última actualización: 03:02:37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1181
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:02:37</t>
+          <t>Última actualización: 04:03:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -478,21 +478,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:02:37</t>
+          <t>04:03:21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -503,21 +503,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:02:37</t>
+          <t>04:03:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,21 +528,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:02:37</t>
+          <t>04:03:21</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,23 +553,98 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:02:37</t>
+          <t>04:03:21</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D9" t="n">
+        <v>79</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>91</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>103</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>05:54</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>111</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -581,6 +656,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 30/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 04:03:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>43</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>91</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -597,14 +789,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 30/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 30/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:02:37</t>
+          <t>Última actualización: 04:03:21</t>
         </is>
       </c>
     </row>
@@ -645,65 +837,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:02:37</t>
+          <t>04:03:21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 30/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 03:02:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 0</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1182
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:03:21</t>
+          <t>Última actualización: 04:48:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,9 +642,234 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:04</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>76</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>83</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06:14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>86</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>93</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>99</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>101</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>103</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>116</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>118</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -661,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,14 +904,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:03:21</t>
+          <t>Última actualización: 04:48:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -745,7 +970,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:03:21</t>
+          <t>04:48:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -759,9 +984,59 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>83</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>118</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -778,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -796,14 +1071,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:03:21</t>
+          <t>Última actualización: 04:48:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -837,25 +1112,100 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05:43</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>55</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>04:03:21</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>05:44</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>101</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:08</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>80</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:48:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>104</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1183
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:48</t>
+          <t>Última actualización: 05:20:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -578,21 +578,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:23</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,21 +603,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -628,21 +628,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:54</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -653,21 +653,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -678,21 +678,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -703,21 +703,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,21 +728,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,21 +753,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,21 +778,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,21 +828,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,23 +853,173 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>84</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>06:46</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>118</v>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="D22" t="n">
+        <v>86</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>99</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>105</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>107</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>111</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>115</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -886,7 +1036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,14 +1054,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:48</t>
+          <t>Última actualización: 05:20:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -970,7 +1120,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -984,7 +1134,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -995,7 +1145,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1009,7 +1159,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1020,7 +1170,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1034,9 +1184,34 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>111</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1053,7 +1228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,14 +1246,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:48:48</t>
+          <t>Última actualización: 05:20:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1287,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1126,7 +1301,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1162,7 +1337,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1176,7 +1351,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1187,7 +1362,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:48:48</t>
+          <t>05:20:44</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1201,11 +1376,36 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>99</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1184
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:20:44</t>
+          <t>Última actualización: 06:03:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -778,7 +778,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -853,7 +853,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -903,7 +903,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -928,21 +928,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,21 +953,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,23 +1003,273 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>68</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>07:15</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>115</v>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D28" t="n">
+        <v>72</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>78</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>80</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>88</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>88</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>89</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>93</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>96</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>104</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>108</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1036,7 +1286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,14 +1304,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:20:44</t>
+          <t>Última actualización: 06:03:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1395,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1159,7 +1409,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1170,7 +1420,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1184,7 +1434,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1195,7 +1445,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1209,9 +1459,34 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>108</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1228,7 +1503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1246,14 +1521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:20:44</t>
+          <t>Última actualización: 06:03:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1612,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1351,7 +1626,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1362,7 +1637,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:03:38</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1376,7 +1651,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1404,6 +1679,56 @@
         <v>99</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>57</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>92</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1185
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:03:38</t>
+          <t>Última actualización: 06:52:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -903,12 +903,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -933,16 +933,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,21 +953,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -978,21 +978,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1003,21 +1003,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1028,21 +1028,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1053,21 +1053,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1103,21 +1103,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1128,21 +1128,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1153,21 +1153,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,21 +1178,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1208,16 +1208,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,23 +1253,273 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>44</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>47</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>55</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>07:51</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>215D_EL PATO</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>108</v>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="D40" t="n">
+        <v>59</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>74</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>80</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>89</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>90</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>91</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>95</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>110</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1281,223 +1531,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 30/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 06:03:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>04:03:21</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>04:46</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>43</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:20:44</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>05:34</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>14</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:03:38</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>06:11</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:03:38</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>06:46</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>43</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>06:03:38</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>68</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>06:03:38</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>07:51</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>108</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1514,14 +1547,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 30/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 30/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:03:38</t>
+          <t>Última actualización: 06:52:41</t>
         </is>
       </c>
     </row>
@@ -1562,6 +1595,248 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>04:03:21</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>04:46</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>43</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05:20:44</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:03:38</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>43</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>19</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>59</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>91</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 30/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 06:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>05:20:44</t>
         </is>
       </c>
@@ -1662,7 +1937,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:20:44</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1676,7 +1951,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1712,7 +1987,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1726,9 +2001,59 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>74</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:52:41</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:31</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>99</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1186
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:41</t>
+          <t>Última actualización: 07:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1183,16 +1183,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06:03:38</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1253,21 +1253,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1278,21 +1278,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1303,21 +1303,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1328,21 +1328,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1353,21 +1353,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1378,21 +1378,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1403,21 +1403,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1428,21 +1428,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1483,16 +1483,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,23 +1503,348 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>49</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>58</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>59</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>60</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>64</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>06:52:41</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D52" t="n">
         <v>110</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>80</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>81</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>91</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>98</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>107</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>113</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>118</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>119</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1536,7 +1861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1554,14 +1879,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:41</t>
+          <t>Última actualización: 07:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1720,7 +2045,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1734,7 +2059,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1745,7 +2070,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1759,9 +2084,34 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1778,7 +2128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1796,14 +2146,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:41</t>
+          <t>Última actualización: 07:23:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -1987,7 +2337,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2001,7 +2351,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2037,25 +2387,100 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:09</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>46</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>06:52:41</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>08:31</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>99</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>72</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:23:38</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>105</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1187
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:23:38</t>
+          <t>Última actualización: 07:59:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 67</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1428,7 +1428,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1478,21 +1478,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1503,21 +1503,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:04</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1528,21 +1528,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1553,21 +1553,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1578,21 +1578,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1603,21 +1603,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1628,21 +1628,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1653,21 +1653,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1678,21 +1678,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:34</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1783,16 +1783,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1803,21 +1803,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,23 +1828,323 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>55</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>62</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>64</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>71</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>77</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>81</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>82</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>09:22</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>119</v>
-      </c>
-      <c r="E60" t="inlineStr">
+      <c r="D67" t="n">
+        <v>83</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>84</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>93</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>94</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>102</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>104</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1861,7 +2161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1879,14 +2179,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:23:38</t>
+          <t>Última actualización: 07:59:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2370,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2084,7 +2384,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2095,7 +2395,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2109,9 +2409,34 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>102</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2128,7 +2453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2146,14 +2471,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:23:38</t>
+          <t>Última actualización: 07:59:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -2412,37 +2737,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:31</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2451,7 +2776,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2462,23 +2787,48 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>36</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>09:08</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>105</v>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="D18" t="n">
+        <v>69</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1188
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:59:51</t>
+          <t>Última actualización: 08:31:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 67</t>
+          <t>Total filas: 83</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1703,21 +1703,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:34</t>
+          <t>08:32</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:34</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1753,21 +1753,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1778,12 +1778,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1808,16 +1808,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1828,21 +1828,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,21 +1853,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:44</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1878,21 +1878,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1903,21 +1903,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1958,16 +1958,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,21 +1978,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2033,16 +2033,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2083,16 +2083,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2103,21 +2103,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2133,18 +2133,418 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>09:20</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>81</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>50</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>83</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>52</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>84</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09:24</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>53</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>61</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>62</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>09:35</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>64</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>102</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>71</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>07:59:51</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D72" t="n">
+      <c r="D83" t="n">
         <v>104</v>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>73</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>101</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>110</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>111</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>115</v>
+      </c>
+      <c r="E88" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2161,7 +2561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2179,14 +2579,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:59:51</t>
+          <t>Última actualización: 08:31:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2795,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2409,7 +2809,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2437,6 +2837,56 @@
         <v>102</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>71</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>115</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2453,7 +2903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2471,14 +2921,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:59:51</t>
+          <t>Última actualización: 08:31:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -2812,25 +3262,100 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:37</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>07:59:51</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>09:08</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>69</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>38</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>92</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1189
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:31:16</t>
+          <t>Última actualización: 08:54:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 83</t>
+          <t>Total filas: 93</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1903,7 +1903,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1928,21 +1928,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1953,21 +1953,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1978,12 +1978,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2028,21 +2028,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2053,21 +2053,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2078,21 +2078,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2108,16 +2108,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2128,21 +2128,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09:20</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2153,21 +2153,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2178,21 +2178,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2203,21 +2203,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,21 +2228,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2253,21 +2253,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,21 +2278,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,21 +2303,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2353,21 +2353,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2378,21 +2378,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2403,21 +2403,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,21 +2428,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,21 +2453,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2483,16 +2483,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2503,21 +2503,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2533,18 +2533,268 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>71</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>49</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>73</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>58</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>59</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>101</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>08:31:16</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>110</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>88</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
           <t>10:26</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C96" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>115</v>
-      </c>
-      <c r="E88" t="inlineStr">
+      <c r="D96" t="n">
+        <v>92</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>10:41</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>107</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>109</v>
+      </c>
+      <c r="E98" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2579,7 +2829,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:31:16</t>
+          <t>Última actualización: 08:54:41</t>
         </is>
       </c>
     </row>
@@ -2820,7 +3070,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2834,7 +3084,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2870,7 +3120,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2884,7 +3134,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2903,7 +3153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2921,14 +3171,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:31:16</t>
+          <t>Última actualización: 08:54:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3312,7 +3562,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3326,7 +3576,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3337,23 +3587,48 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>08:54:41</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>68</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>08:31:16</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D22" t="n">
         <v>92</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1190
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:41</t>
+          <t>Última actualización: 09:32:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 93</t>
+          <t>Total filas: 107</t>
         </is>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2403,7 +2403,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2503,7 +2503,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2553,21 +2553,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2578,12 +2578,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2603,21 +2603,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2628,21 +2628,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:46</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2653,12 +2653,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2678,21 +2678,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2703,21 +2703,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>09:54</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2728,21 +2728,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:03</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2753,21 +2753,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>10:41</t>
+          <t>10:04</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2778,23 +2778,373 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>40</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>41</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>49</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>50</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>51</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>54</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>10:41</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>69</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
           <t>10:43</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D98" t="n">
+      <c r="D105" t="n">
+        <v>71</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>81</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>89</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>94</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>107</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
         <v>109</v>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>114</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>115</v>
+      </c>
+      <c r="E112" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2811,7 +3161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2829,14 +3179,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:41</t>
+          <t>Última actualización: 09:32:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3420,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3084,7 +3434,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -3120,7 +3470,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3134,9 +3484,34 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>89</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3153,7 +3528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3171,14 +3546,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:54:41</t>
+          <t>Última actualización: 09:32:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3962,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3601,7 +3976,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3631,6 +4006,56 @@
       <c r="E22" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>82</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>101</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1191
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:32:47</t>
+          <t>Última actualización: 10:39:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 107</t>
+          <t>Total filas: 135</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2928,21 +2928,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>10:41</t>
+          <t>10:40</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2958,16 +2958,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:41</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2978,21 +2978,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>10:53</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3008,16 +3008,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3028,21 +3028,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>10:47</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3053,21 +3053,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3078,21 +3078,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3108,16 +3108,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3128,23 +3128,723 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>18</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>18</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
           <t>09:32:47</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>89</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>23</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>25</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>11:05</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>26</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>94</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>11:07</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>28</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>32</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>11:12</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>33</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>107</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>11:20</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>41</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>42</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>09:32:47</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>114</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
         <is>
           <t>11:27</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
+      <c r="C126" t="inlineStr">
         <is>
           <t>225_C ROCA-H SUR</t>
         </is>
       </c>
-      <c r="D112" t="n">
-        <v>115</v>
-      </c>
-      <c r="E112" t="inlineStr">
+      <c r="D126" t="n">
+        <v>48</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>11:32</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>53</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>56</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>11:36</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>57</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>63</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>64</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>72</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>80</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>83</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>12:07</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>88</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>95</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>102</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>102</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>103</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>118</v>
+      </c>
+      <c r="E140" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3161,7 +3861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3179,14 +3879,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:32:47</t>
+          <t>Última actualización: 10:39:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -3512,6 +4212,81 @@
         <v>89</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>23</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>72</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>102</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3528,7 +4303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3546,14 +4321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:32:47</t>
+          <t>Última actualización: 10:39:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -4012,7 +4787,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4026,7 +4801,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4056,6 +4831,56 @@
       <c r="E24" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>35</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>85</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1192
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:39:14</t>
+          <t>Última actualización: 11:19:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 135</t>
+          <t>Total filas: 155</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3378,7 +3378,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3428,7 +3428,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3453,21 +3453,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>11:22</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3478,21 +3478,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,21 +3503,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3528,21 +3528,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3553,21 +3553,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>11:36</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3578,21 +3578,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3603,21 +3603,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3633,16 +3633,16 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,21 +3653,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:36</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3683,16 +3683,16 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:36</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3703,21 +3703,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3728,21 +3728,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>11:43</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3753,21 +3753,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3778,21 +3778,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3803,21 +3803,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3833,18 +3833,518 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>83</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>45</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>47</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>47</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>47</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:07</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>88</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>12:13</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>54</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>55</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>61</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>61</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>102</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>62</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>103</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>77</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10:39:14</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
           <t>12:37</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr">
+      <c r="C154" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D140" t="n">
+      <c r="D154" t="n">
         <v>118</v>
       </c>
-      <c r="E140" t="inlineStr">
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>79</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>82</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>89</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>91</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>107</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>115</v>
+      </c>
+      <c r="E160" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3861,7 +4361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3879,14 +4379,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:39:14</t>
+          <t>Última actualización: 11:19:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4745,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4259,7 +4759,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -4270,23 +4770,73 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>61</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>10:39:14</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>12:21</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>102</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>115</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4303,7 +4853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4321,14 +4871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:39:14</t>
+          <t>Última actualización: 11:19:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -4862,7 +5412,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4876,11 +5426,36 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:19:35</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>94</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1193
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:19:35</t>
+          <t>Última actualización: 11:57:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 155</t>
+          <t>Total filas: 167</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3817,7 +3817,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -3978,21 +3978,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4003,21 +4003,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4028,21 +4028,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:14</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4053,21 +4053,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4078,21 +4078,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4103,21 +4103,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4133,16 +4133,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,21 +4153,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4183,16 +4183,16 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4203,21 +4203,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:26</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,23 +4328,323 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>41</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>44</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>51</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>53</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>65</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>13:06</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>69</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
           <t>13:14</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr">
+      <c r="C166" t="inlineStr">
         <is>
           <t>215D_EL PATO</t>
         </is>
       </c>
-      <c r="D160" t="n">
-        <v>115</v>
-      </c>
-      <c r="E160" t="inlineStr">
+      <c r="D166" t="n">
+        <v>77</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>84</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>84</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>89</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>109</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>113</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>119</v>
+      </c>
+      <c r="E172" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4361,7 +4661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4379,14 +4679,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:19:35</t>
+          <t>Última actualización: 11:57:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -4770,7 +5070,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4784,7 +5084,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -4820,7 +5120,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4834,9 +5134,34 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>113</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4853,7 +5178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4871,14 +5196,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:19:35</t>
+          <t>Última actualización: 11:57:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5412,7 +5737,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5426,7 +5751,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -5437,7 +5762,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5451,11 +5776,36 @@
         </is>
       </c>
       <c r="D27" t="n">
+        <v>56</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>94</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>L6203</t>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1194
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:57:34</t>
+          <t>Última actualización: 12:30:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 167</t>
+          <t>Total filas: 182</t>
         </is>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4228,21 +4228,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:31</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4253,21 +4253,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4278,21 +4278,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4303,21 +4303,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4328,21 +4328,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4358,16 +4358,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,21 +4378,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4403,21 +4403,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4428,21 +4428,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4453,21 +4453,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4483,16 +4483,16 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4503,21 +4503,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,21 +4528,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,21 +4578,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4608,16 +4608,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,23 +4628,398 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>49</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
           <t>11:57:34</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>84</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>51</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>56</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>56</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>13:41</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>71</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>76</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>76</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>80</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>85</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
         <is>
           <t>13:56</t>
         </is>
       </c>
-      <c r="C172" t="inlineStr">
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>86</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>11:57:34</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D172" t="n">
+      <c r="D183" t="n">
         <v>119</v>
       </c>
-      <c r="E172" t="inlineStr">
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>94</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>106</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>109</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>111</v>
+      </c>
+      <c r="E187" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4661,7 +5036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4679,14 +5054,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:57:34</t>
+          <t>Última actualización: 12:30:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -5120,12 +5495,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -5134,7 +5509,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -5150,18 +5525,68 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>77</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>13:50</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>113</v>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="D24" t="n">
+        <v>80</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>109</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5178,7 +5603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5196,14 +5621,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:57:34</t>
+          <t>Última actualización: 12:30:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -5762,7 +6187,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -5776,7 +6201,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -5787,23 +6212,73 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>60</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>11:57:34</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>13:31</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D29" t="n">
         <v>94</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:30:50</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>99</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1195
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E187"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:30:50</t>
+          <t>Última actualización: 13:02:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 182</t>
+          <t>Total filas: 194</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4553,21 +4553,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,21 +4578,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,21 +4603,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,21 +4628,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>13:19</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,21 +4653,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,21 +4678,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4708,16 +4708,16 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4728,21 +4728,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4753,21 +4753,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>13:41</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,21 +4778,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,21 +4803,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4828,21 +4828,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4853,21 +4853,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>13:55</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4878,21 +4878,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:34</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4903,21 +4903,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4933,16 +4933,16 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:41</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4953,21 +4953,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4978,21 +4978,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5003,23 +5003,323 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>48</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>48</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
           <t>12:30:50</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>85</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>54</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>54</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>62</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>14:06</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>64</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>74</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>77</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
         <is>
           <t>14:21</t>
         </is>
       </c>
-      <c r="C187" t="inlineStr">
+      <c r="C196" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D187" t="n">
-        <v>111</v>
-      </c>
-      <c r="E187" t="inlineStr">
+      <c r="D196" t="n">
+        <v>79</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>114</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>116</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>118</v>
+      </c>
+      <c r="E199" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5036,7 +5336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5054,14 +5354,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:30:50</t>
+          <t>Última actualización: 13:02:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -5495,7 +5795,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -5509,7 +5809,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -5545,7 +5845,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -5559,7 +5859,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -5570,7 +5870,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -5584,9 +5884,34 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>116</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5603,7 +5928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5621,14 +5946,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:30:50</t>
+          <t>Última actualización: 13:02:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -6237,7 +6562,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -6251,7 +6576,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -6262,7 +6587,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6276,11 +6601,36 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>110</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1196
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:02:37</t>
+          <t>Última actualización: 13:55:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 194</t>
+          <t>Total filas: 214</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5053,7 +5053,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5128,21 +5128,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5153,21 +5153,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>14:06</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5178,21 +5178,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5208,16 +5208,16 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5228,21 +5228,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5253,21 +5253,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:12</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5283,16 +5283,16 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5303,23 +5303,523 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>22</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
           <t>13:02:37</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>77</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>25</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>26</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>32</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>14:28</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>33</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>50</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>13:02:37</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>114</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>14:57</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>62</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>63</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
         <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="C199" t="inlineStr">
+      <c r="C209" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D199" t="n">
-        <v>118</v>
-      </c>
-      <c r="E199" t="inlineStr">
+      <c r="D209" t="n">
+        <v>65</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>70</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>15:10</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>75</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>79</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>15:26</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>91</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>100</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>102</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>104</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>109</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>112</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>119</v>
+      </c>
+      <c r="E219" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5336,7 +5836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5354,14 +5854,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:02:37</t>
+          <t>Última actualización: 13:55:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5895,23 +6395,73 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>25</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>14:58</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>116</v>
-      </c>
-      <c r="E26" t="inlineStr">
+      <c r="D27" t="n">
+        <v>63</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>104</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5928,7 +6478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5946,14 +6496,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:02:37</t>
+          <t>Última actualización: 13:55:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -6587,7 +7137,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -6601,7 +7151,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -6631,6 +7181,56 @@
       <c r="E31" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>58</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>99</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1197
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:55:05</t>
+          <t>Última actualización: 14:26:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 214</t>
+          <t>Total filas: 232</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5403,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:26</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5428,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>14:28</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5453,21 +5453,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5478,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:35</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5503,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>14:57</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:44</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5558,16 +5558,16 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5578,21 +5578,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:46</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5633,16 +5633,16 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>15:26</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,12 +5703,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5783,16 +5783,16 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,23 +5803,473 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>55</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
           <t>13:55:05</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>15:26</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>91</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>66</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>100</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>71</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>72</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>72</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>104</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>15:44</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>109</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>79</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>80</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>112</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>87</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>87</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
         <is>
           <t>15:54</t>
         </is>
       </c>
-      <c r="C219" t="inlineStr">
+      <c r="C233" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D219" t="n">
+      <c r="D233" t="n">
         <v>119</v>
       </c>
-      <c r="E219" t="inlineStr">
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>90</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>109</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>114</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>115</v>
+      </c>
+      <c r="E237" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5836,7 +6286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5854,14 +6304,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:55:05</t>
+          <t>Última actualización: 14:26:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -6420,7 +6870,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -6434,7 +6884,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -6445,23 +6895,73 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>72</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>13:55:05</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>15:39</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D29" t="n">
         <v>104</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>114</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6478,7 +6978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6496,14 +6996,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:55:05</t>
+          <t>Última actualización: 14:26:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -7187,7 +7687,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7201,7 +7701,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -7212,7 +7712,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7226,11 +7726,36 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>108</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1198
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E237"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:26:27</t>
+          <t>Última actualización: 14:57:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 232</t>
+          <t>Total filas: 246</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4513,11 +4513,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,21 +5653,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5678,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5703,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5728,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5753,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5778,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5803,21 +5803,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5828,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>15:26</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5858,16 +5858,16 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5883,16 +5883,16 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5903,21 +5903,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5928,21 +5928,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:26</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,21 +5953,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5978,21 +5978,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6008,16 +6008,16 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6058,16 +6058,16 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>119</v>
+        <v>48</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6233,16 +6233,16 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,23 +6253,373 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>56</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>13:55:05</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>119</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>58</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>59</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
           <t>14:26:27</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>90</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>16:08</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>71</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>78</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>82</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>114</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
         <is>
           <t>16:21</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr">
+      <c r="C246" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D237" t="n">
-        <v>115</v>
-      </c>
-      <c r="E237" t="inlineStr">
+      <c r="D246" t="n">
+        <v>84</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>93</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>105</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>106</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>111</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>119</v>
+      </c>
+      <c r="E251" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6286,7 +6636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6304,14 +6654,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:26:27</t>
+          <t>Última actualización: 14:57:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -6870,7 +7220,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -6884,7 +7234,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -6895,7 +7245,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -6909,7 +7259,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -6945,23 +7295,48 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>82</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>14:26:27</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>16:20</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D31" t="n">
         <v>114</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6978,7 +7353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6996,14 +7371,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:26:27</t>
+          <t>Última actualización: 14:57:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -7712,7 +8087,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7726,7 +8101,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -7737,25 +8112,75 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:13</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>76</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>14:26:27</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>16:14</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D35" t="n">
         <v>108</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:57:41</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>115</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1199
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:41</t>
+          <t>Última actualización: 15:37:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 246</t>
+          <t>Total filas: 259</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4513,11 +4513,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6092,7 +6092,7 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>15:39</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:39</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,21 +6178,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:44</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6203,21 +6203,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6228,21 +6228,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6253,21 +6253,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6278,21 +6278,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,21 +6303,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,21 +6328,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,21 +6353,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:54</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6383,16 +6383,16 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6428,21 +6428,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6483,16 +6483,16 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6533,16 +6533,16 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,21 +6553,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6578,21 +6578,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,23 +6603,348 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>52</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>53</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>59</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>16:38</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>61</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>63</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>65</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>66</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>71</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>16:50</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>73</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="C251" t="inlineStr">
+      <c r="C260" t="inlineStr">
         <is>
           <t>17_179 Y 38</t>
         </is>
       </c>
-      <c r="D251" t="n">
+      <c r="D260" t="n">
+        <v>79</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>87</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>104</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>107</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
         <v>119</v>
       </c>
-      <c r="E251" t="inlineStr">
+      <c r="E264" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6636,7 +6961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6654,14 +6979,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:41</t>
+          <t>Última actualización: 15:37:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -7245,7 +7570,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -7259,7 +7584,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -7320,7 +7645,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -7334,9 +7659,34 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>87</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7353,7 +7703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7371,14 +7721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:57:41</t>
+          <t>Última actualización: 15:37:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -8137,7 +8487,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -8151,7 +8501,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -8179,6 +8529,56 @@
         <v>115</v>
       </c>
       <c r="E36" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>76</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>15:37:31</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>17:14</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>97</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1200
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E278"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:37:31</t>
+          <t>Última actualización: 16:18:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 259</t>
+          <t>Total filas: 273</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,7 +6103,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -6113,11 +6113,11 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6578,7 +6578,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:26</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6628,21 +6628,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6653,21 +6653,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6678,21 +6678,21 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>16:38</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6703,21 +6703,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6733,16 +6733,16 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6758,16 +6758,16 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:38</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6783,16 +6783,16 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6803,21 +6803,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6828,21 +6828,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6853,21 +6853,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,23 +6928,373 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>39</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>46</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>46</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>46</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>17:16</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>58</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>63</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>66</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>70</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>74</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
           <t>15:37:31</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
+      <c r="B273" t="inlineStr">
         <is>
           <t>17:36</t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
+      <c r="C273" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D264" t="n">
+      <c r="D273" t="n">
         <v>119</v>
       </c>
-      <c r="E264" t="inlineStr">
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>80</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>82</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>92</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>94</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>106</v>
+      </c>
+      <c r="E278" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6961,7 +7311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6979,14 +7329,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:37:31</t>
+          <t>Última actualización: 16:18:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -7620,7 +7970,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -7634,7 +7984,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -7670,7 +8020,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7684,9 +8034,34 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>82</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7703,7 +8078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7721,14 +8096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:37:31</t>
+          <t>Última actualización: 16:18:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -8512,7 +8887,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8526,7 +8901,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8581,6 +8956,56 @@
       <c r="E38" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>17:20</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>62</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>16:18:44</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>105</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1201
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E278"/>
+  <dimension ref="A1:E289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:44</t>
+          <t>Última actualización: 16:48:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 273</t>
+          <t>Total filas: 284</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6878,21 +6878,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,21 +6903,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6933,16 +6933,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6978,21 +6978,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7033,16 +7033,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,21 +7053,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7153,21 +7153,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,21 +7203,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7283,18 +7283,293 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>74</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>46</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>48</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>50</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>52</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>62</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>64</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>72</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C278" t="inlineStr">
+      <c r="C286" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D278" t="n">
-        <v>106</v>
-      </c>
-      <c r="E278" t="inlineStr">
+      <c r="D286" t="n">
+        <v>76</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>93</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>99</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>104</v>
+      </c>
+      <c r="E289" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7311,7 +7586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7329,14 +7604,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:44</t>
+          <t>Última actualización: 16:48:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -8020,7 +8295,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8034,7 +8309,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -8045,7 +8320,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -8059,9 +8334,34 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>99</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8078,7 +8378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8096,14 +8396,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:44</t>
+          <t>Última actualización: 16:48:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -8887,12 +9187,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -8901,7 +9201,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -8912,12 +9212,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -8926,7 +9226,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -8942,16 +9242,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -8962,12 +9262,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -8976,7 +9276,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -8992,18 +9292,68 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>17:20</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>62</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>33</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>16:48:42</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>18:03</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D40" t="n">
-        <v>105</v>
-      </c>
-      <c r="E40" t="inlineStr">
+      <c r="D42" t="n">
+        <v>75</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1202
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E289"/>
+  <dimension ref="A1:E298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:48:42</t>
+          <t>Última actualización: 17:01:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 284</t>
+          <t>Total filas: 293</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3903,7 +3903,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3913,11 +3913,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D144" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6688,7 +6688,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -7028,21 +7028,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:01</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7053,12 +7053,12 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -7067,7 +7067,7 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7108,16 +7108,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7158,16 +7158,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7178,21 +7178,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7203,21 +7203,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7228,21 +7228,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7253,21 +7253,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,21 +7328,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,21 +7353,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,21 +7453,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,23 +7553,248 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>49</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>51</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
           <t>16:48:42</t>
         </is>
       </c>
-      <c r="B289" t="inlineStr">
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>72</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>63</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>18:08</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>67</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>80</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>86</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
         <is>
           <t>18:32</t>
         </is>
       </c>
-      <c r="C289" t="inlineStr">
+      <c r="C296" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D289" t="n">
-        <v>104</v>
-      </c>
-      <c r="E289" t="inlineStr">
+      <c r="D296" t="n">
+        <v>91</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>107</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>117</v>
+      </c>
+      <c r="E298" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7586,7 +7811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7604,14 +7829,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:48:42</t>
+          <t>Última actualización: 17:01:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -8295,7 +8520,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -8309,7 +8534,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -8320,7 +8545,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -8334,7 +8559,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -8345,7 +8570,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -8359,9 +8584,34 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>117</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8378,7 +8628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8396,14 +8646,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:48:42</t>
+          <t>Última actualización: 17:01:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -9312,7 +9562,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -9326,7 +9576,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -9337,7 +9587,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -9351,11 +9601,36 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17:01:39</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:51</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>110</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1203
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E298"/>
+  <dimension ref="A1:E313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:01:39</t>
+          <t>Última actualización: 17:43:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 293</t>
+          <t>Total filas: 308</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3903,7 +3903,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3913,11 +3913,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6938,11 +6938,11 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6963,11 +6963,11 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7528,21 +7528,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,21 +7628,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:07</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,23 +7778,398 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>33</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>38</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>41</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
           <t>17:01:39</t>
         </is>
       </c>
-      <c r="B298" t="inlineStr">
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>86</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>45</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>49</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>18:34</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>51</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>57</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>65</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
         <is>
           <t>18:58</t>
         </is>
       </c>
-      <c r="C298" t="inlineStr">
+      <c r="C307" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D298" t="n">
+      <c r="D307" t="n">
+        <v>75</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>81</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>87</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>93</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>98</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>107</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
         <v>117</v>
       </c>
-      <c r="E298" t="inlineStr">
+      <c r="E313" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7811,7 +8186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7829,14 +8204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:01:39</t>
+          <t>Última actualización: 17:43:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -8595,23 +8970,73 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>45</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>18:58</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D36" t="n">
+        <v>75</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
         <v>117</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8628,7 +9053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8646,14 +9071,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:01:39</t>
+          <t>Última actualización: 17:43:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -9612,23 +10037,98 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>21</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>17:01:39</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>18:51</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D44" t="n">
         <v>110</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>69</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>81</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1204
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E313"/>
+  <dimension ref="A1:E327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:43:26</t>
+          <t>Última actualización: 18:03:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 308</t>
+          <t>Total filas: 322</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4513,11 +4513,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6688,7 +6688,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -6888,7 +6888,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6938,11 +6938,11 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6963,11 +6963,11 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7703,7 +7703,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -7717,7 +7717,7 @@
         </is>
       </c>
       <c r="D295" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>18:07</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:07</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7783,16 +7783,16 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7883,16 +7883,16 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,21 +7953,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,21 +7978,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8008,16 +8008,16 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,21 +8028,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,21 +8053,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,23 +8153,373 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>55</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
           <t>17:43:26</t>
         </is>
       </c>
-      <c r="B313" t="inlineStr">
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>81</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>62</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>87</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>68</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>17:43:26</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>93</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>74</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>78</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>87</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C313" t="inlineStr">
+      <c r="C322" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D313" t="n">
-        <v>117</v>
-      </c>
-      <c r="E313" t="inlineStr">
+      <c r="D322" t="n">
+        <v>97</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>98</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>107</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>108</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>108</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>116</v>
+      </c>
+      <c r="E327" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8204,7 +8554,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:43:26</t>
+          <t>Última actualización: 18:03:18</t>
         </is>
       </c>
     </row>
@@ -8970,7 +9320,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -8984,7 +9334,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -8995,7 +9345,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -9009,7 +9359,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -9020,7 +9370,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -9034,7 +9384,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -9053,7 +9403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9071,14 +9421,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:43:26</t>
+          <t>Última actualización: 18:03:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -10037,7 +10387,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -10051,7 +10401,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10087,7 +10437,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10101,7 +10451,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -10112,7 +10462,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:03:18</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10126,11 +10476,36 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>18:03:18</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>111</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1205
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E327"/>
+  <dimension ref="A1:E338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:03:18</t>
+          <t>Última actualización: 18:37:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 322</t>
+          <t>Total filas: 333</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4513,11 +4513,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7138,11 +7138,11 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8067,7 +8067,7 @@
         </is>
       </c>
       <c r="D309" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,21 +8078,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8128,21 +8128,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,21 +8153,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8208,16 +8208,16 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,21 +8228,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,21 +8278,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8303,21 +8303,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,21 +8353,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8378,21 +8378,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,21 +8403,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,21 +8453,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,21 +8478,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,23 +8503,298 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>53</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>58</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>63</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>19:41</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>64</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>73</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>74</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>74</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
           <t>19:59</t>
         </is>
       </c>
-      <c r="C327" t="inlineStr">
+      <c r="C334" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D327" t="n">
-        <v>116</v>
-      </c>
-      <c r="E327" t="inlineStr">
+      <c r="D334" t="n">
+        <v>82</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>94</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>105</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>107</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>114</v>
+      </c>
+      <c r="E338" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8536,7 +8811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8554,14 +8829,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:03:18</t>
+          <t>Última actualización: 18:37:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -9370,23 +9645,73 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>22</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>97</v>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="D38" t="n">
+        <v>63</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>107</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9421,7 +9746,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:03:18</t>
+          <t>Última actualización: 18:37:16</t>
         </is>
       </c>
     </row>
@@ -10437,7 +10762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10451,7 +10776,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -10462,7 +10787,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -10476,7 +10801,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10487,7 +10812,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -10501,7 +10826,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1206
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E338"/>
+  <dimension ref="A1:E346"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:16</t>
+          <t>Última actualización: 18:52:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 333</t>
+          <t>Total filas: 341</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6888,11 +6888,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7138,11 +7138,11 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -8153,7 +8153,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8178,21 +8178,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8203,21 +8203,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8228,12 +8228,12 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -8242,7 +8242,7 @@
         </is>
       </c>
       <c r="D316" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8253,21 +8253,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8278,12 +8278,12 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -8292,7 +8292,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8328,21 +8328,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8353,12 +8353,12 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -8367,7 +8367,7 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8383,16 +8383,16 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,21 +8403,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,12 +8428,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>17:43:26</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -8442,7 +8442,7 @@
         </is>
       </c>
       <c r="D324" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,21 +8453,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,12 +8478,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8492,7 +8492,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,21 +8503,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,21 +8528,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8558,16 +8558,16 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,21 +8603,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8683,16 +8683,16 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8703,21 +8703,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8758,16 +8758,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,23 +8778,223 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>59</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>67</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>78</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
           <t>18:37:16</t>
         </is>
       </c>
-      <c r="B338" t="inlineStr">
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>94</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>90</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>91</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>107</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>98</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C338" t="inlineStr">
+      <c r="C346" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D338" t="n">
-        <v>114</v>
-      </c>
-      <c r="E338" t="inlineStr">
+      <c r="D346" t="n">
+        <v>99</v>
+      </c>
+      <c r="E346" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8811,7 +9011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8829,14 +9029,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:16</t>
+          <t>Última actualización: 18:52:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -9620,7 +9820,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18:03:18</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -9634,7 +9834,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -9670,7 +9870,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -9684,7 +9884,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -9695,23 +9895,48 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>91</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>18:37:16</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>20:24</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D40" t="n">
         <v>107</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9728,7 +9953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9746,14 +9971,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:16</t>
+          <t>Última actualización: 18:52:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -10762,7 +10987,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -10776,7 +11001,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -10812,25 +11037,100 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>13</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>18:37:16</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>19:54</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>77</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>19:55</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>63</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>107</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1207
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E346"/>
+  <dimension ref="A1:E366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:19</t>
+          <t>Última actualización: 19:14:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 341</t>
+          <t>Total filas: 361</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4128,7 +4128,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -4138,11 +4138,11 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4163,11 +4163,11 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6888,11 +6888,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8428,21 +8428,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>17:43:26</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:14</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,12 +8453,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -8467,7 +8467,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8483,16 +8483,16 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,21 +8503,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,21 +8528,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,21 +8553,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8583,16 +8583,16 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8608,16 +8608,16 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,21 +8628,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8658,16 +8658,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,21 +8678,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8708,16 +8708,16 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8728,21 +8728,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,21 +8778,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8808,16 +8808,16 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,21 +8828,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8858,16 +8858,16 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8878,21 +8878,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,21 +8903,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,21 +8928,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,23 +8978,523 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>37</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
           <t>18:52:19</t>
         </is>
       </c>
-      <c r="B346" t="inlineStr">
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>67</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>20:02</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>48</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>20:09</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>55</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>56</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>56</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>94</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>20:16</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>62</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>67</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>90</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>69</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18:37:16</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>107</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>76</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>98</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C346" t="inlineStr">
+      <c r="C360" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D346" t="n">
+      <c r="D360" t="n">
         <v>99</v>
       </c>
-      <c r="E346" t="inlineStr">
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>89</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>98</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>101</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>102</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>110</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>113</v>
+      </c>
+      <c r="E366" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9011,7 +9511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9029,14 +9529,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:19</t>
+          <t>Última actualización: 19:14:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -9870,12 +10370,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -9884,7 +10384,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -9900,16 +10400,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -9920,23 +10420,73 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>69</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>18:37:16</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B41" t="inlineStr">
         <is>
           <t>20:24</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D41" t="n">
         <v>107</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>113</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9953,7 +10503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9971,14 +10521,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:19</t>
+          <t>Última actualización: 19:14:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -11112,23 +11662,48 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>45</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>19:14:51</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>107</v>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="D51" t="n">
+        <v>85</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1208
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E366"/>
+  <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:51</t>
+          <t>Última actualización: 19:46:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 361</t>
+          <t>Total filas: 375</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3888,11 +3888,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D143" t="n">
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6888,7 +6888,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D262" t="n">
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7138,11 +7138,11 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -8303,7 +8303,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8313,11 +8313,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,7 +8328,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8338,11 +8338,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8513,7 +8513,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8878,21 +8878,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,12 +8903,12 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8917,7 +8917,7 @@
         </is>
       </c>
       <c r="D343" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,12 +8928,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:47</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8983,16 +8983,16 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9003,21 +9003,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>20:02</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9128,21 +9128,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9158,16 +9158,16 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>20:16</t>
+          <t>20:02</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9233,16 +9233,16 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,21 +9253,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,21 +9278,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9303,21 +9303,21 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,21 +9328,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:16</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9358,7 +9358,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -9367,7 +9367,7 @@
         </is>
       </c>
       <c r="D361" t="n">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,21 +9378,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9403,21 +9403,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9458,16 +9458,16 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,23 +9478,373 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
+          <t>18:52:19</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>98</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>45</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>20:35</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>49</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
           <t>19:14:51</t>
         </is>
       </c>
-      <c r="B366" t="inlineStr">
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>89</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>58</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>66</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>66</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>69</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>70</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>78</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
         <is>
           <t>21:07</t>
         </is>
       </c>
-      <c r="C366" t="inlineStr">
+      <c r="C376" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D366" t="n">
-        <v>113</v>
-      </c>
-      <c r="E366" t="inlineStr">
+      <c r="D376" t="n">
+        <v>81</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>94</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>96</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>111</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>112</v>
+      </c>
+      <c r="E380" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9529,7 +9879,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:51</t>
+          <t>Última actualización: 19:46:36</t>
         </is>
       </c>
     </row>
@@ -10420,7 +10770,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -10434,7 +10784,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -10470,7 +10820,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -10484,7 +10834,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -10503,7 +10853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10521,14 +10871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:14:51</t>
+          <t>Última actualización: 19:46:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -11687,25 +12037,100 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>20:03</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>17</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>19:14:51</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>85</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>20:40</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>54</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>102</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1209
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E380"/>
+  <dimension ref="A1:E390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:36</t>
+          <t>Última actualización: 20:02:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 375</t>
+          <t>Total filas: 385</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6328,7 +6328,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>13:55:05</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>13:55:05</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6853,7 +6853,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6938,11 +6938,11 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6963,11 +6963,11 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -8538,7 +8538,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -9003,7 +9003,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -9013,11 +9013,11 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,7 +9028,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -9038,11 +9038,11 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,7 +9053,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -9063,11 +9063,11 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,7 +9078,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -9088,11 +9088,11 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9178,21 +9178,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>20:02</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:03</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9228,21 +9228,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9258,16 +9258,16 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9278,21 +9278,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9308,16 +9308,16 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9333,16 +9333,16 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>20:16</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9353,21 +9353,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,21 +9378,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9403,21 +9403,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:16</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,21 +9453,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,21 +9478,21 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,21 +9503,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9528,21 +9528,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>20:35</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9558,16 +9558,16 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,21 +9578,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9608,16 +9608,16 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:35</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9628,21 +9628,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,21 +9653,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,21 +9678,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,21 +9703,21 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9733,16 +9733,16 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9758,16 +9758,16 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9833,18 +9833,268 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>81</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>66</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>94</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>79</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D384" t="n">
+        <v>96</v>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>81</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>111</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
           <t>21:38</t>
         </is>
       </c>
-      <c r="C380" t="inlineStr">
+      <c r="C387" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D380" t="n">
-        <v>112</v>
-      </c>
-      <c r="E380" t="inlineStr">
+      <c r="D387" t="n">
+        <v>96</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>96</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>105</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>21:53</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>111</v>
+      </c>
+      <c r="E390" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9861,7 +10111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9879,14 +10129,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:36</t>
+          <t>Última actualización: 20:02:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -10795,7 +11045,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -10809,7 +11059,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -10837,6 +11087,56 @@
         <v>81</v>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>66</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>105</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10853,7 +11153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10871,14 +11171,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:36</t>
+          <t>Última actualización: 20:02:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -12112,23 +12412,73 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>39</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>19:46:36</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B55" t="inlineStr">
         <is>
           <t>21:28</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D55" t="n">
         <v>102</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>20:02:13</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>87</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1210
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E390"/>
+  <dimension ref="A1:E398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:02:13</t>
+          <t>Última actualización: 20:36:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 385</t>
+          <t>Total filas: 393</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2303,7 +2303,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2313,11 +2313,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2338,11 +2338,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4503,7 +4503,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:30:50</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4513,11 +4513,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>12:30:50</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4538,11 +4538,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6878,7 +6878,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6888,11 +6888,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6938,11 +6938,11 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6963,11 +6963,11 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8303,7 +8303,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8313,11 +8313,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,7 +8328,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8338,11 +8338,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8538,7 +8538,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D328" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8803,7 +8803,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -8813,11 +8813,11 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,7 +8828,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -8838,11 +8838,11 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -9053,7 +9053,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -9063,11 +9063,11 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,7 +9078,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -9088,11 +9088,11 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9303,7 +9303,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -9313,11 +9313,11 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,7 +9328,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -9338,11 +9338,11 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9628,21 +9628,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:36</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,12 +9653,12 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
@@ -9667,7 +9667,7 @@
         </is>
       </c>
       <c r="D373" t="n">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,21 +9678,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,7 +9703,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9728,21 +9728,21 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9753,21 +9753,21 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9853,21 +9853,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9883,16 +9883,16 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,21 +9903,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9933,16 +9933,16 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,21 +9953,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9983,16 +9983,16 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,21 +10003,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,21 +10028,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10053,21 +10053,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,23 +10078,223 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>57</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>19:46:36</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>111</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>62</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>62</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>71</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
           <t>21:53</t>
         </is>
       </c>
-      <c r="C390" t="inlineStr">
+      <c r="C395" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D390" t="n">
-        <v>111</v>
-      </c>
-      <c r="E390" t="inlineStr">
+      <c r="D395" t="n">
+        <v>77</v>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>92</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>92</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>112</v>
+      </c>
+      <c r="E398" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10129,7 +10329,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:02:13</t>
+          <t>Última actualización: 20:36:02</t>
         </is>
       </c>
     </row>
@@ -11095,7 +11295,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -11109,7 +11309,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -11120,7 +11320,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -11134,7 +11334,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -11153,7 +11353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11171,14 +11371,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:02:13</t>
+          <t>Última actualización: 20:36:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -12412,7 +12612,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -12426,7 +12626,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -12462,7 +12662,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -12476,11 +12676,36 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>89</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1211
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E398"/>
+  <dimension ref="A1:E411"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:36:02</t>
+          <t>Última actualización: 20:53:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 393</t>
+          <t>Total filas: 406</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1828,7 +1828,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1838,11 +1838,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1863,11 +1863,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3603,7 +3603,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3613,11 +3613,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3638,11 +3638,11 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3903,7 +3903,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3913,11 +3913,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D187" t="n">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D190" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D191" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6928,7 +6928,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -6938,11 +6938,11 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -6963,11 +6963,11 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
@@ -8303,7 +8303,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8313,11 +8313,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8328,7 +8328,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8338,11 +8338,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8513,7 +8513,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D327" t="n">
@@ -8538,7 +8538,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9003,7 +9003,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -9013,11 +9013,11 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9028,7 +9028,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -9038,11 +9038,11 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9303,7 +9303,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -9313,11 +9313,11 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,7 +9328,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -9338,11 +9338,11 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9753,7 +9753,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -9763,11 +9763,11 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9853,21 +9853,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9878,21 +9878,21 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,21 +9903,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9928,21 +9928,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,21 +9953,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9978,21 +9978,21 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,12 +10003,12 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -10017,7 +10017,7 @@
         </is>
       </c>
       <c r="D387" t="n">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,21 +10028,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10053,21 +10053,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,21 +10078,21 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10103,21 +10103,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10133,16 +10133,16 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10158,16 +10158,16 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10178,21 +10178,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10208,16 +10208,16 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10228,21 +10228,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10258,7 +10258,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -10267,7 +10267,7 @@
         </is>
       </c>
       <c r="D397" t="n">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,23 +10278,348 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>45</v>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>21:41</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>48</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>54</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
           <t>20:36:02</t>
         </is>
       </c>
-      <c r="B398" t="inlineStr">
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>21:53</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>77</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>22:07</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>74</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>92</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>92</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>22:22</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>89</v>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>22:22</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>89</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>94</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
         <is>
           <t>22:28</t>
         </is>
       </c>
-      <c r="C398" t="inlineStr">
+      <c r="C408" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D398" t="n">
+      <c r="D408" t="n">
         <v>112</v>
       </c>
-      <c r="E398" t="inlineStr">
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>22:35</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>102</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>106</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>22:48</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>115</v>
+      </c>
+      <c r="E411" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10311,7 +10636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10329,14 +10654,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:36:02</t>
+          <t>Última actualización: 20:53:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -11295,7 +11620,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -11309,7 +11634,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -11320,7 +11645,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -11334,9 +11659,34 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>106</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11353,7 +11703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11371,14 +11721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:36:02</t>
+          <t>Última actualización: 20:53:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
     </row>
@@ -12662,7 +13012,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -12676,7 +13026,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -12687,7 +13037,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -12701,9 +13051,34 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E57" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>20:53:29</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>87</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 1212
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-30.xlsx
+++ b/data/horarios-141-2026-01-30.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E411"/>
+  <dimension ref="A1:E421"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:53:29</t>
+          <t>Última actualización: 22:06:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 406</t>
+          <t>Total filas: 416</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>07:23:38</t>
+          <t>06:52:41</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1178,7 +1178,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:52:41</t>
+          <t>07:23:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2253,7 +2253,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:54:41</t>
+          <t>07:59:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2263,11 +2263,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:59:51</t>
+          <t>08:54:41</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2288,11 +2288,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:31:16</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2538,11 +2538,11 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2553,7 +2553,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>08:31:16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2563,11 +2563,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3088,11 +3088,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3103,7 +3103,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3113,11 +3113,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -3478,7 +3478,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:32:47</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>09:32:47</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3513,11 +3513,11 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3653,7 +3653,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3663,11 +3663,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -3903,7 +3903,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>11:19:35</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3913,11 +3913,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3928,7 +3928,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:19:35</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -4353,7 +4353,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10:39:14</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4363,11 +4363,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>10:39:14</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4388,11 +4388,11 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4688,11 +4688,11 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>13:02:37</t>
+          <t>11:57:34</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:57:34</t>
+          <t>13:02:37</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D208" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -6028,7 +6028,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:57:41</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6038,11 +6038,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:57:41</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6063,11 +6063,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -6088,11 +6088,11 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -6128,7 +6128,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6138,11 +6138,11 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6278,7 +6278,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:37:31</t>
+          <t>14:26:27</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -6288,11 +6288,11 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6303,7 +6303,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>14:26:27</t>
+          <t>15:37:31</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -6313,11 +6313,11 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -6688,7 +6688,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -7078,7 +7078,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>17:01:39</t>
+          <t>16:18:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7088,11 +7088,11 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,7 +7103,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:18:44</t>
+          <t>16:48:42</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -7113,11 +7113,11 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,7 +7128,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:48:42</t>
+          <t>17:01:39</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -7138,11 +7138,11 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
@@ -7488,7 +7488,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -8113,7 +8113,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D312" t="n">
@@ -8578,7 +8578,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:52:19</t>
+          <t>18:37:16</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -8588,11 +8588,11 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:37:16</t>
+          <t>18:52:19</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D342" t="n">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D343" t="n">
@@ -8938,7 +8938,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
@@ -9303,7 +9303,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>19:46:36</t>
+          <t>19:14:51</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -9313,11 +9313,11 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,7 +9328,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>19:14:51</t>
+          <t>19:46:36</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -9338,11 +9338,11 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9703,7 +9703,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:02:13</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9728,7 +9728,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>20:02:13</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -9738,11 +9738,11 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9763,7 +9763,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D377" t="n">
@@ -9788,7 +9788,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D378" t="n">
@@ -10063,7 +10063,7 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D389" t="n">
@@ -10088,7 +10088,7 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D390" t="n">
@@ -10253,7 +10253,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -10263,11 +10263,11 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,7 +10278,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10288,11 +10288,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10378,21 +10378,21 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>22:06</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10403,12 +10403,12 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
@@ -10417,7 +10417,7 @@
         </is>
       </c>
       <c r="D403" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,21 +10428,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,21 +10453,21 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>20:36:02</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10503,21 +10503,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:12</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10528,21 +10528,21 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>20:36:02</t>
+          <t>20:53:29</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>22:35</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10578,21 +10578,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,23 +10603,273 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>21</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>20:36:02</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D412" t="n">
+        <v>112</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>22</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D414" t="n">
+        <v>26</v>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
           <t>20:53:29</t>
         </is>
       </c>
-      <c r="B411" t="inlineStr">
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>22:35</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>102</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>33</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
         <is>
           <t>22:48</t>
         </is>
       </c>
-      <c r="C411" t="inlineStr">
+      <c r="C417" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D411" t="n">
-        <v>115</v>
-      </c>
-      <c r="E411" t="inlineStr">
+      <c r="D417" t="n">
+        <v>42</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>61</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>62</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>100</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>112</v>
+      </c>
+      <c r="E421" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10636,7 +10886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10654,14 +10904,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:53:29</t>
+          <t>Última actualización: 22:06:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -11670,7 +11920,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20:53:29</t>
+          <t>22:06:48</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -11684,9 +11934,34 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>100</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11703,7 +11978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11721,14 +11996,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:53:29</t>
+          <t>Última actualización: 22:06:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -13062,23 +13337,98 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>22:06</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>20:53:29</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D59" t="n">
         <v>87</v>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>22:29</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>23</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>22:06:48</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>61</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>